<commit_message>
Add testcase, keywords and repository
Add testcase, keywords and repository of plant name and PM
</commit_message>
<xml_diff>
--- a/Document/Testcase_Plant.xlsx
+++ b/Document/Testcase_Plant.xlsx
@@ -126,9 +126,6 @@
     <t>Plant Name is required</t>
   </si>
   <si>
-    <t>Delete a company and its associated list of machines and locations</t>
-  </si>
-  <si>
     <t>the machines and locations itself are NOT deleted</t>
   </si>
   <si>
@@ -202,6 +199,9 @@
   </si>
   <si>
     <t>Code textbox must be empty</t>
+  </si>
+  <si>
+    <t>Delete a Plant and its associated list of machines and locations</t>
   </si>
 </sst>
 </file>
@@ -1328,7 +1328,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1338,8 +1338,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:I34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -1411,17 +1411,17 @@
         <v>2</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D6" s="4" t="s">
         <v>9</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F6" s="4"/>
       <c r="G6" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H6" s="4"/>
       <c r="I6" s="4"/>
@@ -1431,17 +1431,17 @@
         <v>3</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D7" s="4" t="s">
         <v>9</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F7" s="4"/>
       <c r="G7" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H7" s="4"/>
       <c r="I7" s="4"/>
@@ -1451,7 +1451,7 @@
         <v>4</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D8" s="4" t="s">
         <v>9</v>
@@ -1459,7 +1459,7 @@
       <c r="E8" s="4"/>
       <c r="F8" s="4"/>
       <c r="G8" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="H8" s="4"/>
       <c r="I8" s="4"/>
@@ -1533,7 +1533,7 @@
       <c r="E12" s="4"/>
       <c r="F12" s="4"/>
       <c r="G12" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="H12" s="4"/>
       <c r="I12" s="4"/>
@@ -1727,13 +1727,13 @@
         <v>19</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>35</v>
+        <v>60</v>
       </c>
       <c r="D23" s="4" t="s">
         <v>6</v>
       </c>
       <c r="E23" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F23" s="4"/>
       <c r="G23" s="4" t="s">
@@ -1747,7 +1747,7 @@
         <v>20</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D24" s="4" t="s">
         <v>6</v>
@@ -1765,7 +1765,7 @@
         <v>21</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D25" s="4" t="s">
         <v>9</v>
@@ -1773,7 +1773,7 @@
       <c r="E25" s="4"/>
       <c r="F25" s="4"/>
       <c r="G25" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H25" s="4"/>
       <c r="I25" s="4"/>
@@ -1783,7 +1783,7 @@
         <v>22</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D26" s="4" t="s">
         <v>9</v>
@@ -1791,7 +1791,7 @@
       <c r="E26" s="4"/>
       <c r="F26" s="4"/>
       <c r="G26" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H26" s="4"/>
       <c r="I26" s="4"/>
@@ -1801,7 +1801,7 @@
         <v>23</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D27" s="4" t="s">
         <v>9</v>
@@ -1819,7 +1819,7 @@
         <v>24</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D28" s="4" t="s">
         <v>6</v>
@@ -1837,7 +1837,7 @@
         <v>25</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D29" s="4" t="s">
         <v>6</v>
@@ -1855,7 +1855,7 @@
         <v>26</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D30" s="4" t="s">
         <v>6</v>
@@ -1873,7 +1873,7 @@
         <v>27</v>
       </c>
       <c r="C31" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D31" s="4" t="s">
         <v>9</v>
@@ -1881,7 +1881,7 @@
       <c r="E31" s="4"/>
       <c r="F31" s="4"/>
       <c r="G31" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H31" s="4"/>
       <c r="I31" s="4"/>
@@ -1891,7 +1891,7 @@
         <v>28</v>
       </c>
       <c r="C32" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D32" s="4" t="s">
         <v>9</v>
@@ -1899,7 +1899,7 @@
       <c r="E32" s="4"/>
       <c r="F32" s="4"/>
       <c r="G32" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H32" s="4"/>
       <c r="I32" s="4"/>
@@ -1909,7 +1909,7 @@
         <v>29</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D33" s="4" t="s">
         <v>6</v>
@@ -1927,7 +1927,7 @@
         <v>30</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D34" s="4" t="s">
         <v>6</v>

</xml_diff>